<commit_message>
fix to kits bulk operation
</commit_message>
<xml_diff>
--- a/public/operacao-em-massa-kits.xlsx
+++ b/public/operacao-em-massa-kits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\OneDrive - AMPERE ENERGIAS\Área de Trabalho\crm-ampere-2.0\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCDAB03-82DF-478C-87C1-29142D8CE05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB29F790-FDE2-4270-9192-50E8FE2B7DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CADASTRO" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>NOME</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>SERVIÇO 2</t>
+  </si>
+  <si>
+    <t>VISIBILIDADE DE PARCEIRO</t>
   </si>
 </sst>
 </file>
@@ -578,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y37"/>
+  <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,14 +592,14 @@
     <col min="1" max="1" width="30.77734375" style="2" customWidth="1"/>
     <col min="2" max="2" width="30.77734375" style="7" customWidth="1"/>
     <col min="3" max="4" width="30.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.77734375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="35.88671875" style="7" customWidth="1"/>
-    <col min="7" max="24" width="30.77734375" style="2" customWidth="1"/>
-    <col min="25" max="25" width="20.44140625" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="8.88671875" style="2"/>
+    <col min="5" max="6" width="30.77734375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="35.88671875" style="7" customWidth="1"/>
+    <col min="8" max="25" width="30.77734375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="20.44140625" style="2" customWidth="1"/>
+    <col min="27" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -613,67 +616,70 @@
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>20</v>
       </c>
@@ -686,191 +692,191 @@
       <c r="E2" s="7">
         <v>35000</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>45657</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>550</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>10</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>12</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="V2" s="2">
+      <c r="W2" s="2">
         <v>1</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="X2" s="2">
+      <c r="Y2" s="2">
         <v>5</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="G3" s="3"/>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="G4" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="G5" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="G6" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="G7" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="G8" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="G9" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H9" s="3"/>
-      <c r="K9" s="4"/>
-      <c r="Q9" s="4"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="G10" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="L9" s="4"/>
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="G11" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="G12" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="G13" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="G14" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="G15" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="G16" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G17" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G18" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G19" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G20" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G21" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G22" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G23" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G24" s="3"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G25" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G26" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G27" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G28" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G29" s="3"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G30" s="3"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G31" s="3"/>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G32" s="3"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D33" s="4"/>
-      <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G34" s="3"/>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G35" s="3"/>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G36" s="3"/>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G37" s="3"/>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -882,7 +888,7 @@
           <x14:formula1>
             <xm:f>DADOS!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
+          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{56B778B4-F36C-4D0B-BB63-5D894CD542F8}">
           <x14:formula1>
@@ -900,7 +906,7 @@
           <x14:formula1>
             <xm:f>DADOS!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I1048576 O2:O1048576</xm:sqref>
+          <xm:sqref>J2:J1048576 P2:P1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7C80B07A-8E86-4EC2-A15F-ABA9AFACE28A}">
           <x14:formula1>
@@ -912,7 +918,7 @@
           <x14:formula1>
             <xm:f>DADOS!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>Y2:Y1048576</xm:sqref>
+          <xm:sqref>Z2:Z1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>